<commit_message>
Add new Shortcuts and set default terminal
</commit_message>
<xml_diff>
--- a/visual-code-shortcuts.xlsx
+++ b/visual-code-shortcuts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vezeto\custom-configs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Dani\Documents\custom-configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="116">
   <si>
     <t>Ctrl</t>
   </si>
@@ -125,9 +125,6 @@
     <t xml:space="preserve"> Save File</t>
   </si>
   <si>
-    <t>Save As</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -239,6 +236,27 @@
     </r>
   </si>
   <si>
+    <t>Fuzzy search</t>
+  </si>
+  <si>
+    <t>Quick open</t>
+  </si>
+  <si>
+    <t>Show Debug</t>
+  </si>
+  <si>
+    <t>Show Explorer</t>
+  </si>
+  <si>
+    <t>Find in Files</t>
+  </si>
+  <si>
+    <t>Replace in files</t>
+  </si>
+  <si>
+    <t>Select all matched</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -248,7 +266,29 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Toggle tab move </t>
+      <t>Toggle problems</t>
+    </r>
+  </si>
+  <si>
+    <t>New window</t>
+  </si>
+  <si>
+    <t>Go to Symbol in file</t>
+  </si>
+  <si>
+    <t>Show all commands</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
     </r>
     <r>
       <rPr>
@@ -259,17 +299,11 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/ Toggle Menu</t>
-    </r>
-  </si>
-  <si>
-    <t>Fuzzy search</t>
-  </si>
-  <si>
-    <t>Quick open</t>
-  </si>
-  <si>
-    <t>Open recent</t>
+      <t>/ Reload Window</t>
+    </r>
+  </si>
+  <si>
+    <t>Save As / Save All</t>
   </si>
   <si>
     <r>
@@ -281,12 +315,273 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Toggle output</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Format Uppercase</t>
+    </r>
+  </si>
+  <si>
+    <t>Show Extensions</t>
+  </si>
+  <si>
+    <t>Redo</t>
+  </si>
+  <si>
+    <t>- / Format Document</t>
+  </si>
+  <si>
+    <t>- / Open Terminal</t>
+  </si>
+  <si>
+    <t>Show Git</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Close Window </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Close All Files</t>
+    </r>
+  </si>
+  <si>
+    <t>Toggle tab move / Toggle Menu</t>
+  </si>
+  <si>
+    <t>Shift+Alt</t>
+  </si>
+  <si>
+    <t>↑</t>
+  </si>
+  <si>
+    <t>→</t>
+  </si>
+  <si>
+    <t>↓</t>
+  </si>
+  <si>
+    <t>←</t>
+  </si>
+  <si>
+    <t>Select word left</t>
+  </si>
+  <si>
+    <t>Select word right</t>
+  </si>
+  <si>
+    <t>Move word left</t>
+  </si>
+  <si>
+    <t>Move word right</t>
+  </si>
+  <si>
+    <t>Move line up</t>
+  </si>
+  <si>
+    <t>Move line down</t>
+  </si>
+  <si>
+    <t>Expand selection</t>
+  </si>
+  <si>
+    <t>Collapse selection</t>
+  </si>
+  <si>
+    <t>Open Markdown preview</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run Build Task </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Jump to bracket</t>
+    </r>
+  </si>
+  <si>
+    <t>Organize imports</t>
+  </si>
+  <si>
+    <t>Open External Terminal</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Change All Occurrences</t>
+    </r>
+  </si>
+  <si>
+    <t>Toggle block comment</t>
+  </si>
+  <si>
+    <t>Toggle Git Lens</t>
+  </si>
+  <si>
+    <t>Copy file path</t>
+  </si>
+  <si>
+    <t>Show branch history</t>
+  </si>
+  <si>
+    <t>Add cursors to line end</t>
+  </si>
+  <si>
+    <t>Reveal file in OS</t>
+  </si>
+  <si>
+    <t>Add cursor below</t>
+  </si>
+  <si>
+    <t>Add cursor above</t>
+  </si>
+  <si>
+    <t>Move editor next group</t>
+  </si>
+  <si>
+    <t>Move editor previous group</t>
+  </si>
+  <si>
+    <r>
+      <t>Scroll up</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Add prev find to selection</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Scroll down  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Add next find to selection</t>
+    </r>
+  </si>
+  <si>
+    <t>Move prev find to last selection</t>
+  </si>
+  <si>
+    <t>Move next find to last selection</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Organize imports</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add line to selection </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Import NPM module</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuzzy search </t>
+  </si>
+  <si>
+    <t>- / Wrap in Emmet</t>
+  </si>
+  <si>
+    <t>- / Format Lowercase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- / Clear All Notifications </t>
+  </si>
+  <si>
+    <t>- / Duplicate editor to the side</t>
+  </si>
+  <si>
+    <t>- / Convert indentation to tabs</t>
+  </si>
+  <si>
+    <t>- / Run NPM script</t>
+  </si>
+  <si>
+    <t>- / Save As</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve"> Go to symbol </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="238"/>
@@ -294,143 +589,6 @@
       </rPr>
       <t>/ Search on Google</t>
     </r>
-  </si>
-  <si>
-    <t>- /Format Lowercase</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-</t>
-    </r>
-  </si>
-  <si>
-    <t>Run Build Task</t>
-  </si>
-  <si>
-    <t>Open New Comman Prompt</t>
-  </si>
-  <si>
-    <t>Show Debug</t>
-  </si>
-  <si>
-    <t>Show Explorer</t>
-  </si>
-  <si>
-    <t>Find in Files</t>
-  </si>
-  <si>
-    <t>Replace in files</t>
-  </si>
-  <si>
-    <t>Select all matched</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Toggle problems</t>
-    </r>
-  </si>
-  <si>
-    <t>New window</t>
-  </si>
-  <si>
-    <t>Go to Symbol in file</t>
-  </si>
-  <si>
-    <t>Show all commands</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/ Reload Window</t>
-    </r>
-  </si>
-  <si>
-    <t>Save As / Save All</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Toggle output</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> / Format Uppercase</t>
-    </r>
-  </si>
-  <si>
-    <t>Show Extensions</t>
-  </si>
-  <si>
-    <t>Redo</t>
-  </si>
-  <si>
-    <t>- / Format Document</t>
-  </si>
-  <si>
-    <t>- / Open Terminal</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Close Window</t>
-    </r>
-  </si>
-  <si>
-    <t>Show Git</t>
   </si>
 </sst>
 </file>
@@ -500,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -536,6 +694,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -818,21 +986,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="7" max="10" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -843,8 +1014,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -852,59 +1026,77 @@
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E2" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="D3" s="10"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E3" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -912,11 +1104,13 @@
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D7" s="10"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E7" s="5"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -924,11 +1118,12 @@
         <v>13</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -936,73 +1131,85 @@
         <v>15</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E9" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>53</v>
+      <c r="B14" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1010,11 +1217,12 @@
         <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D15" s="9"/>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -1022,47 +1230,58 @@
         <v>26</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E17" s="5"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="9"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E18" s="5"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
@@ -1070,97 +1289,167 @@
         <v>32</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="E21" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="11"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="9"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="9"/>
+      <c r="B29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>